<commit_message>
Edit, mom's substitude schedules added
</commit_message>
<xml_diff>
--- a/Time Table Aug 2018.xlsx
+++ b/Time Table Aug 2018.xlsx
@@ -415,16 +415,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11573,6 +11573,103 @@
               <a:schemeClr val="bg1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>434339</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="217" name="สี่เหลี่ยมผืนผ้า 216"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9753601" y="5812971"/>
+          <a:ext cx="2884714" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ให้แม่ไปรับยาแทนเรา ที่รพนวมินทร์ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t> ใบนัด </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>(3 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดือน</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>บอกอาการ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ให้บัตร</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> ปชช. ของเราไปด้วย</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14360,8 +14457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14370,17 +14467,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13">
         <v>4500</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>42</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -14390,56 +14487,56 @@
       <c r="L1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="16">
+      <c r="O1" s="13">
         <v>20</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="16">
+      <c r="S1" s="13">
         <v>70</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="16">
+      <c r="W1" s="13">
         <v>65</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Y1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="Z1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="16">
+      <c r="AA1" s="13">
         <v>70</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AC1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AD1" s="16">
+      <c r="AD1" s="13">
         <f>((S1+W1)*O1) + AA1</f>
         <v>2770</v>
       </c>
@@ -14460,116 +14557,116 @@
       <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16" t="s">
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="13">
         <v>4</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="16">
+      <c r="S2" s="13">
         <v>50</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="16">
+      <c r="W2" s="13">
         <v>46</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="X2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16" t="s">
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16" t="s">
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="16">
+      <c r="AD2" s="13">
         <f>((S2+W2)*O2)</f>
         <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15">
         <v>0.2</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
         <f>ROUND(F9*(20/100),0)</f>
         <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15">
         <v>0.2</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <f>ROUND(F9*(20/100),0)</f>
         <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15">
         <v>0.2</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
         <f>ROUND(F9*(20/100),0)</f>
         <v>269</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17">
+      <c r="K5" s="14"/>
+      <c r="L5" s="14">
         <f>SUM(H3:H5)+H7</f>
         <v>1076</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="17">
+      <c r="P5" s="14">
         <f>L5</f>
         <v>1076</v>
       </c>
@@ -14591,7 +14688,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="19">
+      <c r="F6" s="16">
         <v>0.15</v>
       </c>
       <c r="G6" s="6"/>
@@ -14601,17 +14698,17 @@
       </c>
     </row>
     <row r="7" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15">
         <v>0.2</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
         <f>ROUND(F9*(20/100),0)</f>
         <v>269</v>
       </c>
@@ -14626,7 +14723,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="19">
+      <c r="F8" s="16">
         <v>0.05</v>
       </c>
       <c r="G8" s="6"/>
@@ -14644,18 +14741,18 @@
       </c>
     </row>
     <row r="9" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
         <f>H1-H9</f>
         <v>1346</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13">
         <f>AD1+AD2</f>
         <v>3154</v>
       </c>
@@ -14675,32 +14772,32 @@
       <c r="A11" s="1">
         <v>43313</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="14"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="19"/>
     </row>
     <row r="12" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -14987,32 +15084,32 @@
       <c r="A21" s="1">
         <v>43313</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="14"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="19"/>
     </row>
     <row r="22" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -15301,32 +15398,32 @@
       <c r="A31" s="1">
         <v>43313</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="13"/>
-      <c r="V31" s="13"/>
-      <c r="W31" s="13"/>
-      <c r="X31" s="13"/>
-      <c r="Y31" s="14"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="18"/>
+      <c r="V31" s="18"/>
+      <c r="W31" s="18"/>
+      <c r="X31" s="18"/>
+      <c r="Y31" s="19"/>
     </row>
     <row r="32" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -15613,32 +15710,32 @@
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="13"/>
-      <c r="V41" s="13"/>
-      <c r="W41" s="13"/>
-      <c r="X41" s="13"/>
-      <c r="Y41" s="14"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="18"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="19"/>
     </row>
     <row r="42" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -16902,32 +16999,32 @@
       <c r="B3" s="1">
         <v>43313</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="14"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="19"/>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
ADDED 6 BASIC NEEDS OFLIVING THINGS WITH AWARENESS, *****VERY NOBLELY IMPORTANT*****
</commit_message>
<xml_diff>
--- a/Time Table Aug 2018.xlsx
+++ b/Time Table Aug 2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="600" windowWidth="15036" windowHeight="6036"/>
+    <workbookView xWindow="420" yWindow="600" windowWidth="11580" windowHeight="5088"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10447,24 +10447,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>32656</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>65314</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>413658</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="213" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6672942" y="5812972"/>
+      <xdr:colOff>32657</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="214" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6640285" y="6302829"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10510,24 +10510,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>10887</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="214" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6640285" y="6302829"/>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="215" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6683828" y="6738257"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10573,24 +10573,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>43542</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>43543</xdr:rowOff>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>32656</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>43543</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="215" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6683828" y="6738257"/>
+      <xdr:rowOff>435428</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="216" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6651171" y="7173685"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10636,24 +10636,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>10885</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>32656</xdr:rowOff>
+      <xdr:colOff>65313</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>43543</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>435428</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="216" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6651171" y="7173685"/>
+      <xdr:colOff>97971</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>413658</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="218" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705599" y="10276115"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10699,24 +10699,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>65313</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:colOff>32656</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>97971</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>413658</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="218" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6705599" y="10276115"/>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="219" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6672942" y="10765972"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10762,24 +10762,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>32656</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>65314</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>10887</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="219" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6672942" y="10765972"/>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="220" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6716485" y="11201400"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10825,24 +10825,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>43543</xdr:rowOff>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>108857</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="220" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6716485" y="11201400"/>
+      <xdr:rowOff>435429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="221" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6683828" y="11636828"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10888,24 +10888,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>43542</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:colOff>32657</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>435429</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="221" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6683828" y="11636828"/>
+      <xdr:colOff>65315</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>402772</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="222" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6672943" y="14282057"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10951,24 +10951,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
+      <xdr:colOff>87085</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>435429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>65315</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>402772</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="222" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6672943" y="14282057"/>
+      <xdr:colOff>119743</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>391887</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="223" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6727371" y="14717486"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11014,24 +11014,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>87085</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>435429</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>119743</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>391887</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="223" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6727371" y="14717486"/>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="224" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6694714" y="15207343"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11077,24 +11077,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>54428</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:colOff>97971</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>87086</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>435429</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="224" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6694714" y="15207343"/>
+      <xdr:colOff>130629</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>424543</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="225" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6738257" y="15642771"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11140,24 +11140,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>97971</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>130629</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>424543</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="225" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6738257" y="15642771"/>
+      <xdr:colOff>97972</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>413657</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="226" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="16078199"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11202,25 +11202,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>65314</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>10885</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>642257</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>97972</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>413657</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="226" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6705600" y="16078199"/>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>413659</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="227" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6618514" y="18756087"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11265,25 +11265,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>642257</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>10887</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>32656</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>413659</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="227" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6618514" y="18756087"/>
+      <xdr:colOff>65314</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>402774</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="228" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6672942" y="19191516"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11329,24 +11329,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>32656</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>32657</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>65314</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>402774</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="228" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6672942" y="19191516"/>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="229" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6640285" y="19681373"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11392,24 +11392,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>43544</xdr:rowOff>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="229" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6640285" y="19681373"/>
+      <xdr:rowOff>435430</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="230" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6683828" y="20116801"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11455,24 +11455,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>43542</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>32658</xdr:rowOff>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>21772</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>435430</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="230" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6683828" y="20116801"/>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>424544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="231" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6651171" y="20552229"/>
           <a:ext cx="6008915" cy="402772"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11515,34 +11515,131 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>32658</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>65313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>261258</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>42453</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="217" name="สี่เหลี่ยมผืนผ้า 216"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10657115" y="5867399"/>
+          <a:ext cx="2884714" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ให้แม่ไปรับยาแทนเรา ที่รพนวมินทร์ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t> ใบนัด </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>(3 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดือน</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t>บอกอาการ </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ให้บัตร</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
+            <a:t> ปชช. ของเราไปด้วย</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>10885</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>21772</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>43543</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>424544</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="231" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6651171" y="20552229"/>
-          <a:ext cx="6008915" cy="402772"/>
+      <xdr:colOff>348343</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>105595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>544287</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>40281</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="234" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6988629" y="7692938"/>
+          <a:ext cx="4180115" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="E46C0A"/>
+          <a:srgbClr val="00B050"/>
         </a:solidFill>
         <a:ln w="25560">
           <a:solidFill>
@@ -11555,51 +11652,776 @@
         <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ไปเล่นเกมส์ที่มหาลัย</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr>
             <a:lnSpc>
               <a:spcPct val="100000"/>
             </a:lnSpc>
           </a:pPr>
-          <a:r>
-            <a:rPr lang="th-TH">
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>587828</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>557349</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16330</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="235" name="สี่เหลี่ยมผืนผ้า 234"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5900057" y="7630887"/>
+          <a:ext cx="633549" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>เดินทาง</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>134503</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>436098</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="236" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3646714" y="7620001"/>
+          <a:ext cx="471960" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>468085</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>478970</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33326</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="237" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3124199" y="6324600"/>
+          <a:ext cx="674914" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ฝาก</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>653143</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>381002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>642257</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>358142</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="238" name="สี่เหลี่ยมผืนผ้า 237"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11277600" y="7522031"/>
+          <a:ext cx="1981200" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ค้นหาเรื่องเที่ยวญี่ปุ่น</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>370114</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>51166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>566058</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>432166</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="239" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010400" y="8084823"/>
+          <a:ext cx="4180115" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>เล่นเกมส์เล็กๆ</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43545</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>20685</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="240" name="สี่เหลี่ยมผืนผ้า 239"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11299372" y="8077202"/>
+          <a:ext cx="1981200" cy="423454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000"/>
+            <a:t>ค้นหาเรื่องเที่ยวญี่ปุ่น</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>206829</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>413660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>489856</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>370785</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="241" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2862943" y="7108374"/>
+          <a:ext cx="947056" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
+              <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>สหกิจ</a:t>
-          </a:r>
-          <a:endParaRPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>เอากลับมา</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH" sz="1000">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
             </a:solidFill>
+            <a:effectLst/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457201</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>402771</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>446313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>468086</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>424542</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="242" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3058885" y="6694713"/>
+          <a:ext cx="729344" cy="424543"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="th-TH" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>ฝาก</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>43542</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>413658</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>515502</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>370784</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="243" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3363685" y="5323115"/>
+          <a:ext cx="471960" cy="403440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="77933C"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>คอมใหญ่</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>323309</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>587829</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>257995</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="244" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16023772" y="5232766"/>
+          <a:ext cx="1164771" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>erect dom</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>315686</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>388624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>10885</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>21772</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>434339</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="217" name="สี่เหลี่ยมผืนผ้า 216"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9753601" y="5812971"/>
-          <a:ext cx="2884714" cy="423454"/>
+      <xdr:rowOff>323309</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="245" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16252372" y="5744395"/>
+          <a:ext cx="1164771" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln w="25560">
+          <a:solidFill>
+            <a:srgbClr val="3A5F8B"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>erect sub</a:t>
+          </a:r>
+          <a:endParaRPr lang="th-TH">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>468085</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>78376</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>445226</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="246" name="สี่เหลี่ยมผืนผ้า 245"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15740742" y="8055428"/>
+          <a:ext cx="938348" cy="423455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11631,114 +12453,8 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ให้แม่ไปรับยาแทนเรา ที่รพนวมินทร์ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>+</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t> ใบนัด </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>(3 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>เดือน</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t>บอกอาการ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ให้บัตร</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> ปชช. ของเราไปด้วย</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>544287</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>435428</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>87086</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>412568</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="232" name="สี่เหลี่ยมผืนผ้า 231"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12496801" y="5344885"/>
-          <a:ext cx="1534885" cy="423454"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000"/>
-            <a:t>ลงทะเบียนสหกิจออนไลน์</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="th-TH" sz="1000" baseline="0"/>
-            <a:t> ใน </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t>regis</a:t>
-          </a:r>
-          <a:endParaRPr lang="th-TH" sz="1000"/>
+            <a:t>ตรวจปฎิทิน</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14527,7 +15243,7 @@
   <dimension ref="A1:AE1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15148,7 +15864,9 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+    </row>
     <row r="21" spans="1:25" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43313</v>

</xml_diff>